<commit_message>
text colors fix, physics system
</commit_message>
<xml_diff>
--- a/assets/CPC Video Memory Pixel converter.xlsx
+++ b/assets/CPC Video Memory Pixel converter.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/retro/proyectos/gemQuest3/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D0BC66-290F-CF4D-931C-D795CB1BF4C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2172840-A568-1D44-B2FF-6BBCD9DDB79A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode 0" sheetId="1" r:id="rId1"/>
     <sheet name="Mode 1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Mode 1'!$B$28:$E$44</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Pixel 1</t>
   </si>
@@ -49,9 +52,6 @@
     <t>MODE 0 Pixel Converter</t>
   </si>
   <si>
-    <t>FF</t>
-  </si>
-  <si>
     <t>White (15)</t>
   </si>
   <si>
@@ -64,42 +64,15 @@
     <t>XX</t>
   </si>
   <si>
-    <t>3C</t>
-  </si>
-  <si>
-    <t>F0</t>
-  </si>
-  <si>
     <t>Blue (12)</t>
   </si>
   <si>
     <t>Mauve (13)</t>
   </si>
   <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>5D</t>
-  </si>
-  <si>
-    <t>1C</t>
-  </si>
-  <si>
     <t>Red (4)</t>
   </si>
   <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>X0</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
     <t>ea</t>
   </si>
   <si>
@@ -208,15 +181,6 @@
     <t>0000</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>0011</t>
-  </si>
-  <si>
-    <t>0111</t>
-  </si>
-  <si>
     <t>White</t>
   </si>
   <si>
@@ -230,13 +194,82 @@
   </si>
   <si>
     <t>0010</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>11111111</t>
+  </si>
+  <si>
+    <t>00001111</t>
+  </si>
+  <si>
+    <t>2X</t>
+  </si>
+  <si>
+    <t>0X</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>c0</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>; CPC Plus Palette - #000,#FFF,#0F0,#00F,#0FF,#666,#060,#6F0,#FF0,#F00,#600,#660,#F0F,#66F,#066,#006</t>
+  </si>
+  <si>
+    <t>; CPC Palette - #54,#4B,#4C,#55,#4D,#40,#5C,#4E,#4A,#52,#56,#5E,#53,#5F,#58,#44</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>Sombra</t>
+  </si>
+  <si>
+    <t>; Graphic Data - 1 Sprites, Mode 0, Width 3 bytes (6 pixels), Height 5, Encoding Screen</t>
+  </si>
+  <si>
+    <t>db #ff,#94,#94,#ff,#94,#94,#ff,#94,#94,#ff,#03,#3c</t>
+  </si>
+  <si>
+    <t>db #ff,#94,#7d</t>
+  </si>
+  <si>
+    <t>X2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,8 +313,14 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +348,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -407,14 +452,46 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,21 +797,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:U23"/>
+  <dimension ref="B1:U36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
+    <col min="4" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
@@ -746,6 +820,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -756,31 +835,46 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="H3" s="29">
+        <v>40</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f>HEX2BIN(MID(H3,1,1),4)&amp;HEX2BIN(MID(H3,2,1),4)</f>
+        <v>01000000</v>
+      </c>
+      <c r="J3" s="3" t="str">
+        <f>BIN2HEX(MID(I3,7,1)&amp;MID(I3,3,1)&amp;MID(I3,5,1)&amp;MID(I3,1,1),2)&amp;" - "&amp;BIN2HEX(MID(I3,8,1)&amp;MID(I3,4,1)&amp;MID(I3,6,1)&amp;MID(I3,2,1),2)</f>
+        <v>00 - 01</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>15</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4</v>
-      </c>
-      <c r="F4" s="7">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>25</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E4" s="30">
+        <v>94</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="H4" s="29">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="str">
+        <f t="shared" ref="I4:I11" si="0">HEX2BIN(MID(H4,1,1),4)&amp;HEX2BIN(MID(H4,2,1),4)</f>
+        <v>00101000</v>
+      </c>
+      <c r="J4" s="3" t="str">
+        <f t="shared" ref="J4:J11" si="1">BIN2HEX(MID(I4,7,1)&amp;MID(I4,3,1)&amp;MID(I4,5,1)&amp;MID(I4,1,1),2)&amp;" - "&amp;BIN2HEX(MID(I4,8,1)&amp;MID(I4,4,1)&amp;MID(I4,6,1)&amp;MID(I4,2,1),2)</f>
+        <v>06 - 00</v>
+      </c>
+      <c r="L4" s="8"/>
       <c r="M4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
@@ -790,47 +884,42 @@
       </c>
       <c r="C5" s="3" t="str">
         <f>DEC2BIN(C4,4)</f>
-        <v>1111</v>
-      </c>
-      <c r="E5" t="str">
-        <f>HEX2BIN(E4,4)</f>
-        <v>0100</v>
-      </c>
-      <c r="F5" t="str">
-        <f>HEX2BIN(F4,4)</f>
-        <v>0010</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5">
-        <v>55</v>
-      </c>
-      <c r="L5" t="s">
-        <v>21</v>
+        <v>0001</v>
+      </c>
+      <c r="E5" s="31" t="str">
+        <f>HEX2BIN(E4,8)</f>
+        <v>10010100</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="H5" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>01101000</v>
+      </c>
+      <c r="J5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>06 - 01</v>
       </c>
       <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="J6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6">
-        <v>55</v>
-      </c>
-      <c r="L6" t="s">
-        <v>30</v>
+      <c r="H6" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>11000000</v>
+      </c>
+      <c r="J6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>01 - 01</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
@@ -843,79 +932,154 @@
       <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7">
-        <v>10</v>
-      </c>
-      <c r="L7">
-        <v>35</v>
-      </c>
-      <c r="M7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7">
-        <v>30</v>
+      <c r="H7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>10010100</v>
+      </c>
+      <c r="J7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>01 - 06</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="str">
-        <f>BIN2HEX(B9,1)</f>
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="str">
-        <f>BIN2HEX(C9,1)</f>
-        <v>5</v>
-      </c>
+      <c r="B8" s="32" t="str">
+        <f>BIN2HEX(MID(B5,4,1)&amp;MID(C5,4,1)&amp;MID(B5,2,1)&amp;MID(C5,2,1)&amp;MID(B5,3,1)&amp;MID(C5,3,1)&amp;MID(B5,1,1)&amp;MID(C5,1,1),2)</f>
+        <v>40</v>
+      </c>
+      <c r="C8" s="32"/>
       <c r="E8" s="1">
-        <f>BIN2DEC(E9)</f>
+        <f>BIN2DEC(MID(E5,7,1)&amp;MID(E5,3,1)&amp;MID(E5,5,1)&amp;MID(E5,1,1))</f>
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <f>BIN2DEC(F9)</f>
-        <v>8</v>
+        <f>BIN2DEC(MID(E5,8,1)&amp;MID(E5,4,1)&amp;MID(E5,6,1)&amp;MID(E5,2,1))</f>
+        <v>6</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>00111100</v>
+      </c>
+      <c r="J8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>06 - 06</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="str">
-        <f>MID(B5,1,1)&amp;MID(C5,1,1)&amp;MID(B5,3,1)&amp;MID(C5,3,1)</f>
-        <v>0101</v>
-      </c>
-      <c r="C9" s="1" t="str">
-        <f>MID(B5,2,1)&amp;MID(C5,2,1)&amp;MID(B5,4,1)&amp;MID(C5,4,1)</f>
-        <v>0101</v>
-      </c>
+      <c r="B9" s="32" t="str">
+        <f>HEX2BIN(B8,8)</f>
+        <v>01000000</v>
+      </c>
+      <c r="C9" s="32"/>
       <c r="E9" s="1" t="str">
-        <f>MID(E5,1,1)&amp;MID(F5,1,1)&amp;MID(E5,3,1)&amp;MID(F5,3,1)</f>
+        <f>DEC2BIN(E8,4)</f>
         <v>0001</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f>MID(E5,2,1)&amp;MID(F5,2,1)&amp;MID(E5,4,1)&amp;MID(F5,4,1)</f>
-        <v>1000</v>
-      </c>
+        <f>DEC2BIN(F8,4)</f>
+        <v>0110</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>00000011</v>
+      </c>
+      <c r="J9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>08 - 08</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="H10" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>01010110</v>
+      </c>
+      <c r="J10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>08 - 07</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="H11" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>01101100</v>
+      </c>
+      <c r="J11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>06 - 03</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="D12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="7">
         <v>6</v>
       </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>47</v>
+      <c r="D13" s="33" t="str">
+        <f>DEC2BIN(C13,4)&amp;1111</f>
+        <v>01101111</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="33" t="str">
+        <f>1111&amp;DEC2BIN(C13,4)</f>
+        <v>11110110</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -928,30 +1092,29 @@
       <c r="U13" s="13"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="3">
-        <v>58</v>
-      </c>
-      <c r="F14" s="3">
-        <v>19</v>
-      </c>
-      <c r="G14" s="3">
-        <v>18</v>
-      </c>
-      <c r="H14" s="3">
-        <v>59</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>48</v>
-      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
+        <v>68</v>
+      </c>
+      <c r="E14" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
+        <v>C0</v>
+      </c>
+      <c r="F14" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
+        <v>94</v>
+      </c>
+      <c r="G14" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
+        <v>40</v>
+      </c>
+      <c r="H14" s="3"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
@@ -963,30 +1126,29 @@
       <c r="U14" s="13"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7">
         <v>8</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="3">
-        <v>33</v>
-      </c>
-      <c r="G15" s="3">
-        <v>30</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>49</v>
-      </c>
+      <c r="D15" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
+        <v>29</v>
+      </c>
+      <c r="E15" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
+        <v>03</v>
+      </c>
+      <c r="F15" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
+        <v>16</v>
+      </c>
+      <c r="G15" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
+        <v>01</v>
+      </c>
+      <c r="H15" s="3"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
@@ -998,30 +1160,29 @@
       <c r="U15" s="13"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="3">
-        <v>28</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="3">
-        <v>22</v>
-      </c>
-      <c r="G16" s="3">
-        <v>20</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7">
+        <v>7</v>
+      </c>
+      <c r="D16" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
+        <v>7C</v>
+      </c>
+      <c r="E16" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
+        <v>FC</v>
+      </c>
+      <c r="F16" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
+        <v>BC</v>
+      </c>
+      <c r="G16" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
+        <v>54</v>
+      </c>
+      <c r="H16" s="3"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
@@ -1033,30 +1194,29 @@
       <c r="U16" s="13"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>55</v>
-      </c>
-      <c r="D17" s="3">
-        <v>14</v>
-      </c>
-      <c r="E17" s="3">
-        <v>50</v>
-      </c>
-      <c r="F17" s="3">
-        <v>11</v>
-      </c>
-      <c r="G17" s="3">
-        <v>10</v>
-      </c>
-      <c r="H17" s="3">
-        <v>51</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3</v>
+      </c>
+      <c r="D17" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
+        <v>6C</v>
+      </c>
+      <c r="E17" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
+        <v>CC</v>
+      </c>
+      <c r="F17" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
+        <v>9C</v>
+      </c>
+      <c r="G17" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
+        <v>44</v>
+      </c>
+      <c r="H17" s="3"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
@@ -1068,8 +1228,27 @@
       <c r="U17" s="13"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="L18" s="14" t="s">
-        <v>52</v>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2</v>
+      </c>
+      <c r="D18" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
+        <v>2C</v>
+      </c>
+      <c r="E18" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
+        <v>0C</v>
+      </c>
+      <c r="F18" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
+        <v>1C</v>
+      </c>
+      <c r="G18" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
+        <v>04</v>
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
@@ -1082,9 +1261,30 @@
       <c r="U18" s="13"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="L19" s="14" t="s">
-        <v>53</v>
-      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7">
+        <v>13</v>
+      </c>
+      <c r="D19" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
+        <v>79</v>
+      </c>
+      <c r="E19" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
+        <v>F3</v>
+      </c>
+      <c r="F19" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
+        <v>B6</v>
+      </c>
+      <c r="G19" s="34" t="str">
+        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
+        <v>51</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
@@ -1096,35 +1296,8 @@
       <c r="U19" s="13"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="D20" t="str">
-        <f>DEC2BIN(B20,4)</f>
-        <v>0000</v>
-      </c>
-      <c r="E20" t="str">
-        <f>DEC2BIN(C20,4)</f>
-        <v>1111</v>
-      </c>
-      <c r="F20" s="1" t="str">
-        <f>MID(D20,1,1)&amp;MID(E20,1,1)&amp;MID(D20,3,1)&amp;MID(E20,3,1)</f>
-        <v>0101</v>
-      </c>
-      <c r="G20" s="1" t="str">
-        <f>MID(D20,2,1)&amp;MID(E20,2,1)&amp;MID(D20,4,1)&amp;MID(E20,4,1)</f>
-        <v>0101</v>
-      </c>
-      <c r="H20" t="str">
-        <f>BIN2HEX(F20)&amp;BIN2HEX(G20)</f>
-        <v>55</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>54</v>
-      </c>
+      <c r="H20" s="28"/>
+      <c r="I20" s="11"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
@@ -1136,35 +1309,11 @@
       <c r="U20" s="13"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>15</v>
-      </c>
-      <c r="C21">
-        <v>7</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" ref="D21:D23" si="0">DEC2BIN(B21,4)</f>
-        <v>1111</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" ref="E21:E23" si="1">DEC2BIN(C21,4)</f>
-        <v>0111</v>
-      </c>
-      <c r="F21" s="1" t="str">
-        <f t="shared" ref="F21:F23" si="2">MID(D21,1,1)&amp;MID(E21,1,1)&amp;MID(D21,3,1)&amp;MID(E21,3,1)</f>
-        <v>1011</v>
-      </c>
-      <c r="G21" s="1" t="str">
-        <f t="shared" ref="G21:G23" si="3">MID(D21,2,1)&amp;MID(E21,2,1)&amp;MID(D21,4,1)&amp;MID(E21,4,1)</f>
-        <v>1111</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" ref="H21:H23" si="4">BIN2HEX(F21)&amp;BIN2HEX(G21)</f>
-        <v>BF</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="B21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="11"/>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
@@ -1176,72 +1325,216 @@
       <c r="U21" s="13"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>15</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>0111</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v>1111</v>
-      </c>
-      <c r="F22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>0111</v>
-      </c>
-      <c r="G22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>1111</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="4"/>
-        <v>7F</v>
-      </c>
+      <c r="B22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="28"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>15</v>
-      </c>
-      <c r="C23">
-        <v>15</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>1111</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="1"/>
-        <v>1111</v>
-      </c>
-      <c r="F23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>1111</v>
-      </c>
-      <c r="G23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>1111</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="4"/>
-        <v>FF</v>
-      </c>
+      <c r="B23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="28"/>
+      <c r="I24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="28"/>
+      <c r="I25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B26" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B29" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+    </row>
+    <row r="33" spans="12:21" x14ac:dyDescent="0.2">
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+    </row>
+    <row r="34" spans="12:21" x14ac:dyDescent="0.2">
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+    </row>
+    <row r="35" spans="12:21" x14ac:dyDescent="0.2">
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+    </row>
+    <row r="36" spans="12:21" x14ac:dyDescent="0.2">
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:V26"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1252,13 +1545,14 @@
     <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="21" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
@@ -1269,10 +1563,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -1283,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -1295,21 +1589,21 @@
         <v>4</v>
       </c>
       <c r="H4" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="M4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="P4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
@@ -1319,7 +1613,7 @@
       </c>
       <c r="C5" s="3" t="str">
         <f>DEC2BIN(C4,2)</f>
-        <v>11</v>
+        <v>01</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" ref="D5:E5" si="0">DEC2BIN(D4,2)</f>
@@ -1335,39 +1629,39 @@
       </c>
       <c r="H5" t="str">
         <f>HEX2BIN(H4,4)</f>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="M5">
         <v>55</v>
       </c>
       <c r="N5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="O5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="L6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="M6">
         <v>55</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
@@ -1381,13 +1675,13 @@
         <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="M7">
         <v>10</v>
@@ -1396,7 +1690,7 @@
         <v>35</v>
       </c>
       <c r="O7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="P7">
         <v>30</v>
@@ -1409,7 +1703,7 @@
       </c>
       <c r="C8" s="1" t="str">
         <f>BIN2HEX(C9,1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1419,7 +1713,7 @@
       </c>
       <c r="H8" s="1">
         <f>BIN2DEC(H9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
         <f>BIN2DEC(I9)</f>
@@ -1431,85 +1725,82 @@
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="str">
+      <c r="B9" s="20" t="str">
         <f>MID(B5,2,1)&amp;MID(C5,2,1)&amp;MID(D5,2,1)&amp;MID(E5,2,1)</f>
         <v>0100</v>
       </c>
-      <c r="C9" s="22" t="str">
+      <c r="C9" s="20" t="str">
         <f>MID(B5,1,1)&amp;MID(C5,1,1)&amp;MID(D5,1,1)&amp;MID(E5,1,1)</f>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="G9" s="22" t="str">
+      <c r="G9" s="20" t="str">
         <f>MID(H5,1,1)&amp;MID(G5,1,1)</f>
         <v>00</v>
       </c>
-      <c r="H9" s="22" t="str">
+      <c r="H9" s="20" t="str">
         <f>MID(H5,2,1)&amp;MID(G5,2,1)</f>
-        <v>11</v>
-      </c>
-      <c r="I9" s="22" t="str">
+        <v>01</v>
+      </c>
+      <c r="I9" s="20" t="str">
         <f>MID(H5,3,1)&amp;MID(G5,3,1)</f>
         <v>00</v>
       </c>
-      <c r="J9" s="22" t="str">
+      <c r="J9" s="20" t="str">
         <f>MID(H5,4,1)&amp;MID(G5,4,1)</f>
         <v>00</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="18">
-        <v>1111</v>
-      </c>
-      <c r="E12" s="18">
-        <v>1110</v>
-      </c>
-      <c r="F12" s="18">
-        <v>1100</v>
-      </c>
-      <c r="G12" s="18">
-        <v>1000</v>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>64</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C13" s="17">
         <v>1</v>
       </c>
       <c r="D13" s="16" t="str">
         <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),4,1),2),1,1),2)</f>
-        <v>F0</v>
+        <v>E0</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" ref="E13:M13" si="1">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),4,1),2),1,1),2)</f>
-        <v>E0</v>
+        <v>C0</v>
       </c>
       <c r="F13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>C0</v>
+        <v>A0</v>
       </c>
       <c r="G13" s="16" t="str">
         <f t="shared" si="1"/>
@@ -1517,55 +1808,46 @@
       </c>
       <c r="H13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>00</v>
+        <v>60</v>
       </c>
       <c r="I13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="L13" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="M13" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
+        <v>00</v>
+      </c>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="25"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
       <c r="V13" s="13"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C14" s="17">
         <v>2</v>
       </c>
       <c r="D14" s="16" t="str">
         <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),4,1),2),1,1),2)</f>
-        <v>0F</v>
+        <v>0E</v>
       </c>
       <c r="E14" s="16" t="str">
         <f t="shared" ref="E14:M14" si="2">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),4,1),2),1,1),2)</f>
-        <v>0E</v>
+        <v>0C</v>
       </c>
       <c r="F14" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>0C</v>
+        <v>0A</v>
       </c>
       <c r="G14" s="16" t="str">
         <f t="shared" si="2"/>
@@ -1573,55 +1855,46 @@
       </c>
       <c r="H14" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>00</v>
+        <v>06</v>
       </c>
       <c r="I14" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>01</v>
+        <v>04</v>
       </c>
       <c r="J14" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="K14" s="16" t="str">
         <f t="shared" si="2"/>
-        <v>07</v>
-      </c>
-      <c r="L14" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v>04</v>
-      </c>
-      <c r="M14" s="16" t="str">
-        <f t="shared" si="2"/>
-        <v>02</v>
-      </c>
+        <v>00</v>
+      </c>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="25"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
       <c r="V14" s="13"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C15" s="17">
         <v>3</v>
       </c>
       <c r="D15" s="16" t="str">
         <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),4,1),2),1,1),2)</f>
-        <v>FF</v>
+        <v>EE</v>
       </c>
       <c r="E15" s="16" t="str">
         <f t="shared" ref="E15:L15" si="3">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),4,1),2),1,1),2)</f>
-        <v>EE</v>
+        <v>CC</v>
       </c>
       <c r="F15" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>CC</v>
+        <v>AA</v>
       </c>
       <c r="G15" s="16" t="str">
         <f t="shared" si="3"/>
@@ -1629,35 +1902,26 @@
       </c>
       <c r="H15" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
+        <v>66</v>
       </c>
       <c r="I15" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="J15" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K15" s="16" t="str">
         <f t="shared" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="L15" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="M15" s="16" t="str">
-        <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(M$12,1,$C$15),4,1),2),1,1),2)</f>
-        <v>22</v>
-      </c>
+        <v>00</v>
+      </c>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="25"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
       <c r="V15" s="13"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
@@ -1668,15 +1932,11 @@
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
       <c r="V16" s="13"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
@@ -1684,15 +1944,11 @@
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
       <c r="V17" s="13"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
@@ -1700,15 +1956,11 @@
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
       <c r="V18" s="13"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
@@ -1716,15 +1968,11 @@
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
       <c r="V19" s="13"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B20" s="12" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1740,7 +1988,7 @@
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -1756,7 +2004,7 @@
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -1772,25 +2020,270 @@
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="13">
+        <v>0</v>
+      </c>
+      <c r="C38" s="13">
+        <v>1</v>
+      </c>
+      <c r="D38" s="13">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="13">
+        <v>0</v>
+      </c>
+      <c r="C39" s="13">
+        <v>1</v>
+      </c>
+      <c r="D39" s="13">
+        <v>0</v>
+      </c>
+      <c r="E39" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="13">
+        <v>0</v>
+      </c>
+      <c r="C40" s="13">
+        <v>1</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0</v>
+      </c>
+      <c r="E40" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="13">
+        <v>0</v>
+      </c>
+      <c r="C41" s="13">
+        <v>0</v>
+      </c>
+      <c r="D41" s="13">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="13">
+        <v>0</v>
+      </c>
+      <c r="C42" s="13">
+        <v>0</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
+      <c r="E42" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="13">
+        <v>0</v>
+      </c>
+      <c r="C43" s="13">
+        <v>0</v>
+      </c>
+      <c r="D43" s="13">
+        <v>0</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="13">
+        <v>0</v>
+      </c>
+      <c r="C44" s="13">
+        <v>0</v>
+      </c>
+      <c r="D44" s="13">
+        <v>0</v>
+      </c>
+      <c r="E44" s="13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B28:E44" xr:uid="{D938356A-6A4F-2045-BA9F-923FC2B756A8}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B12:C12"/>
   </mergeCells>

</xml_diff>

<commit_message>
Text fix, TMatchList WIP01
</commit_message>
<xml_diff>
--- a/assets/CPC Video Memory Pixel converter.xlsx
+++ b/assets/CPC Video Memory Pixel converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/retro/proyectos/gemQuest3/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\retro\GemQuest3\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2172840-A568-1D44-B2FF-6BBCD9DDB79A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556554F9-4B53-4C29-A743-05E55CDA7C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode 0" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>Pixel 1</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Orange (5)</t>
   </si>
   <si>
-    <t>XX</t>
-  </si>
-  <si>
     <t>Blue (12)</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>            Scheme 1. Screen pixel format and video memory</t>
   </si>
   <si>
-    <t>______________________________________________________________________</t>
-  </si>
-  <si>
     <t>                      &lt;---- 1  byte ----&gt;</t>
   </si>
   <si>
@@ -211,15 +205,6 @@
     <t>0110</t>
   </si>
   <si>
-    <t>11111111</t>
-  </si>
-  <si>
-    <t>00001111</t>
-  </si>
-  <si>
-    <t>2X</t>
-  </si>
-  <si>
     <t>0X</t>
   </si>
   <si>
@@ -262,7 +247,79 @@
     <t>db #ff,#94,#7d</t>
   </si>
   <si>
-    <t>X2</t>
+    <t>const u8 sp_palette0[16] = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x54, // 0 - 00 - black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x4b, // 1 - 26 - white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x4c, // 2 - 06 - bright red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x55, // 3 - 02 - bright blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x4d, // 4 - 08 - bright magenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x40, // 5 - 13 - white(gray)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x5c, // 6 - 03 - red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x4e, // 7 - 15 - orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x4A, // 8 - 24 - bright yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x52, // 9 - 18 - bright green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x56, // 10 - 09 - green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x5e, // 11 - 12 - yellow (pale green)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x53, // 12 - 20 - bright cyan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x5f, // 13 - 14 - pastel blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x58, // 14 - 04 - magenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0x44, // 15 - 01 - blue</t>
+  </si>
+  <si>
+    <t>x0</t>
+  </si>
+  <si>
+    <t>Vacío</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>xxxx xxxx</t>
+  </si>
+  <si>
+    <t>xxxx 0000</t>
+  </si>
+  <si>
+    <t>0000 xxxx</t>
+  </si>
+  <si>
+    <t>xxxx ssss</t>
+  </si>
+  <si>
+    <t>xs</t>
   </si>
 </sst>
 </file>
@@ -320,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,12 +405,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,10 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -455,26 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,10 +514,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,35 +827,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:U36"/>
+  <dimension ref="B1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" customWidth="1"/>
-    <col min="4" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>HEX2BIN(MID(H2,1,1),4)&amp;HEX2BIN(MID(H2,2,1),4)</f>
+        <v>00111100</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f>BIN2HEX(MID(I2,7,1)&amp;MID(I2,3,1)&amp;MID(I2,5,1)&amp;MID(I2,1,1),2)&amp;" - "&amp;BIN2HEX(MID(I2,8,1)&amp;MID(I2,4,1)&amp;MID(I2,6,1)&amp;MID(I2,2,1),2)</f>
+        <v>06 - 06</v>
+      </c>
       <c r="M2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -835,7 +877,7 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="19">
         <v>40</v>
       </c>
       <c r="I3" s="3" t="str">
@@ -847,21 +889,21 @@
         <v>00 - 01</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="20">
         <v>94</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="H4" s="29">
+      <c r="F4" s="20"/>
+      <c r="H4" s="19">
         <v>28</v>
       </c>
       <c r="I4" s="3" t="str">
@@ -874,10 +916,10 @@
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>DEC2BIN(B4,4)</f>
         <v>0000</v>
@@ -886,13 +928,13 @@
         <f>DEC2BIN(C4,4)</f>
         <v>0001</v>
       </c>
-      <c r="E5" s="31" t="str">
+      <c r="E5" s="21" t="str">
         <f>HEX2BIN(E4,8)</f>
         <v>10010100</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="H5" s="29" t="s">
-        <v>62</v>
+      <c r="F5" s="21"/>
+      <c r="H5" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -903,12 +945,12 @@
         <v>06 - 01</v>
       </c>
       <c r="M5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="H6" s="29" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H6" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -919,10 +961,10 @@
         <v>01 - 01</v>
       </c>
       <c r="M6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -932,8 +974,8 @@
       <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="29" t="s">
-        <v>64</v>
+      <c r="H7" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -944,12 +986,12 @@
         <v>01 - 06</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B8" s="32" t="str">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="str">
         <f>BIN2HEX(MID(B5,4,1)&amp;MID(C5,4,1)&amp;MID(B5,2,1)&amp;MID(C5,2,1)&amp;MID(B5,3,1)&amp;MID(C5,3,1)&amp;MID(B5,1,1)&amp;MID(C5,1,1),2)</f>
         <v>40</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="22"/>
       <c r="E8" s="1">
         <f>BIN2DEC(MID(E5,7,1)&amp;MID(E5,3,1)&amp;MID(E5,5,1)&amp;MID(E5,1,1))</f>
         <v>1</v>
@@ -958,8 +1000,8 @@
         <f>BIN2DEC(MID(E5,8,1)&amp;MID(E5,4,1)&amp;MID(E5,6,1)&amp;MID(E5,2,1))</f>
         <v>6</v>
       </c>
-      <c r="H8" s="29" t="s">
-        <v>61</v>
+      <c r="H8" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="I8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -970,12 +1012,12 @@
         <v>06 - 06</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B9" s="32" t="str">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="str">
         <f>HEX2BIN(B8,8)</f>
         <v>01000000</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="22"/>
       <c r="E9" s="1" t="str">
         <f>DEC2BIN(E8,4)</f>
         <v>0001</v>
@@ -984,8 +1026,8 @@
         <f>DEC2BIN(F8,4)</f>
         <v>0110</v>
       </c>
-      <c r="H9" s="29" t="s">
-        <v>67</v>
+      <c r="H9" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1002,9 +1044,9 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="H10" s="29" t="s">
-        <v>68</v>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H10" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="I10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1021,9 +1063,9 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="H11" s="29" t="s">
-        <v>69</v>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H11" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1040,412 +1082,484 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="D12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>60</v>
-      </c>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="P12" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="7">
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="25" t="str">
+        <f>DEC2BIN(C15,4)</f>
+        <v>0000</v>
+      </c>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="7">
         <v>6</v>
       </c>
-      <c r="D13" s="33" t="str">
-        <f>DEC2BIN(C13,4)&amp;1111</f>
-        <v>01101111</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="33" t="str">
-        <f>1111&amp;DEC2BIN(C13,4)</f>
-        <v>11110110</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="D16" s="25" t="str">
+        <f>DEC2BIN(C16,4)</f>
+        <v>0110</v>
+      </c>
+      <c r="E16" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D16,4,1)&amp;MID($D$15,2,1)&amp;MID(D16,2,1)&amp;MID($D$15,3,1)&amp;MID(D16,3,1)&amp;MID($D$15,1,1)&amp;MID(D16,1,1),2)</f>
+        <v>0x14</v>
+      </c>
+      <c r="F16" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D16,4,1)&amp;MID($D$15,4,1)&amp;MID(D16,2,1)&amp;MID($D$15,2,1)&amp;MID(D16,3,1)&amp;MID($D$15,3,1)&amp;MID(D16,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0x28</v>
+      </c>
+      <c r="G16" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D16,4,1)&amp;MID(D16,4,1)&amp;MID(D16,2,1)&amp;MID(D16,2,1)&amp;MID(D16,3,1)&amp;MID(D16,3,1)&amp;MID(D16,1,1)&amp;MID(D16,1,1),2)</f>
+        <v>0x3C</v>
+      </c>
+      <c r="H16" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D16,4,1)&amp;MID($D$16,4,1)&amp;MID(D16,2,1)&amp;MID($D$16,2,1)&amp;MID(D16,3,1)&amp;MID($D$16,3,1)&amp;MID(D16,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0x3C</v>
+      </c>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
-        <v>68</v>
-      </c>
-      <c r="E14" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
-        <v>C0</v>
-      </c>
-      <c r="F14" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
-        <v>94</v>
-      </c>
-      <c r="G14" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C14,4)),5,1),2)</f>
-        <v>40</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25" t="str">
+        <f t="shared" ref="D17:D22" si="2">DEC2BIN(C17,4)</f>
+        <v>0001</v>
+      </c>
+      <c r="E17" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D17,4,1)&amp;MID($D$15,2,1)&amp;MID(D17,2,1)&amp;MID($D$15,3,1)&amp;MID(D17,3,1)&amp;MID($D$15,1,1)&amp;MID(D17,1,1),2)</f>
+        <v>0x40</v>
+      </c>
+      <c r="F17" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D17,4,1)&amp;MID($D$15,4,1)&amp;MID(D17,2,1)&amp;MID($D$15,2,1)&amp;MID(D17,3,1)&amp;MID($D$15,3,1)&amp;MID(D17,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0x80</v>
+      </c>
+      <c r="G17" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D17,4,1)&amp;MID(D17,4,1)&amp;MID(D17,2,1)&amp;MID(D17,2,1)&amp;MID(D17,3,1)&amp;MID(D17,3,1)&amp;MID(D17,1,1)&amp;MID(D17,1,1),2)</f>
+        <v>0xC0</v>
+      </c>
+      <c r="H17" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D17,4,1)&amp;MID($D$16,4,1)&amp;MID(D17,2,1)&amp;MID($D$16,2,1)&amp;MID(D17,3,1)&amp;MID($D$16,3,1)&amp;MID(D17,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0x94</v>
+      </c>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C18" s="7">
         <v>8</v>
       </c>
-      <c r="D15" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
-        <v>29</v>
-      </c>
-      <c r="E15" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
-        <v>03</v>
-      </c>
-      <c r="F15" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
-        <v>16</v>
-      </c>
-      <c r="G15" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C15,4)),5,1),2)</f>
-        <v>01</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="D18" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="E18" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D18,4,1)&amp;MID($D$15,2,1)&amp;MID(D18,2,1)&amp;MID($D$15,3,1)&amp;MID(D18,3,1)&amp;MID($D$15,1,1)&amp;MID(D18,1,1),2)</f>
+        <v>0x01</v>
+      </c>
+      <c r="F18" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D18,4,1)&amp;MID($D$15,4,1)&amp;MID(D18,2,1)&amp;MID($D$15,2,1)&amp;MID(D18,3,1)&amp;MID($D$15,3,1)&amp;MID(D18,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0x02</v>
+      </c>
+      <c r="G18" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D18,4,1)&amp;MID(D18,4,1)&amp;MID(D18,2,1)&amp;MID(D18,2,1)&amp;MID(D18,3,1)&amp;MID(D18,3,1)&amp;MID(D18,1,1)&amp;MID(D18,1,1),2)</f>
+        <v>0x03</v>
+      </c>
+      <c r="H18" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D18,4,1)&amp;MID($D$16,4,1)&amp;MID(D18,2,1)&amp;MID($D$16,2,1)&amp;MID(D18,3,1)&amp;MID($D$16,3,1)&amp;MID(D18,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0x16</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C19" s="7">
         <v>7</v>
       </c>
-      <c r="D16" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
-        <v>7C</v>
-      </c>
-      <c r="E16" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
-        <v>FC</v>
-      </c>
-      <c r="F16" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
-        <v>BC</v>
-      </c>
-      <c r="G16" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C16,4)),5,1),2)</f>
-        <v>54</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="D19" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>0111</v>
+      </c>
+      <c r="E19" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D19,4,1)&amp;MID($D$15,2,1)&amp;MID(D19,2,1)&amp;MID($D$15,3,1)&amp;MID(D19,3,1)&amp;MID($D$15,1,1)&amp;MID(D19,1,1),2)</f>
+        <v>0x54</v>
+      </c>
+      <c r="F19" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D19,4,1)&amp;MID($D$15,4,1)&amp;MID(D19,2,1)&amp;MID($D$15,2,1)&amp;MID(D19,3,1)&amp;MID($D$15,3,1)&amp;MID(D19,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0xA8</v>
+      </c>
+      <c r="G19" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D19,4,1)&amp;MID(D19,4,1)&amp;MID(D19,2,1)&amp;MID(D19,2,1)&amp;MID(D19,3,1)&amp;MID(D19,3,1)&amp;MID(D19,1,1)&amp;MID(D19,1,1),2)</f>
+        <v>0xFC</v>
+      </c>
+      <c r="H19" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D19,4,1)&amp;MID($D$16,4,1)&amp;MID(D19,2,1)&amp;MID($D$16,2,1)&amp;MID(D19,3,1)&amp;MID($D$16,3,1)&amp;MID(D19,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0xBC</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <v>3</v>
+      </c>
+      <c r="D20" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>0011</v>
+      </c>
+      <c r="E20" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D20,4,1)&amp;MID($D$15,2,1)&amp;MID(D20,2,1)&amp;MID($D$15,3,1)&amp;MID(D20,3,1)&amp;MID($D$15,1,1)&amp;MID(D20,1,1),2)</f>
+        <v>0x44</v>
+      </c>
+      <c r="F20" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D20,4,1)&amp;MID($D$15,4,1)&amp;MID(D20,2,1)&amp;MID($D$15,2,1)&amp;MID(D20,3,1)&amp;MID($D$15,3,1)&amp;MID(D20,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0x88</v>
+      </c>
+      <c r="G20" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D20,4,1)&amp;MID(D20,4,1)&amp;MID(D20,2,1)&amp;MID(D20,2,1)&amp;MID(D20,3,1)&amp;MID(D20,3,1)&amp;MID(D20,1,1)&amp;MID(D20,1,1),2)</f>
+        <v>0xCC</v>
+      </c>
+      <c r="H20" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D20,4,1)&amp;MID($D$16,4,1)&amp;MID(D20,2,1)&amp;MID($D$16,2,1)&amp;MID(D20,3,1)&amp;MID($D$16,3,1)&amp;MID(D20,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0x9C</v>
+      </c>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2</v>
+      </c>
+      <c r="D21" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>0010</v>
+      </c>
+      <c r="E21" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D21,4,1)&amp;MID($D$15,2,1)&amp;MID(D21,2,1)&amp;MID($D$15,3,1)&amp;MID(D21,3,1)&amp;MID($D$15,1,1)&amp;MID(D21,1,1),2)</f>
+        <v>0x04</v>
+      </c>
+      <c r="F21" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D21,4,1)&amp;MID($D$15,4,1)&amp;MID(D21,2,1)&amp;MID($D$15,2,1)&amp;MID(D21,3,1)&amp;MID($D$15,3,1)&amp;MID(D21,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0x08</v>
+      </c>
+      <c r="G21" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D21,4,1)&amp;MID(D21,4,1)&amp;MID(D21,2,1)&amp;MID(D21,2,1)&amp;MID(D21,3,1)&amp;MID(D21,3,1)&amp;MID(D21,1,1)&amp;MID(D21,1,1),2)</f>
+        <v>0x0C</v>
+      </c>
+      <c r="H21" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D21,4,1)&amp;MID($D$16,4,1)&amp;MID(D21,2,1)&amp;MID($D$16,2,1)&amp;MID(D21,3,1)&amp;MID($D$16,3,1)&amp;MID(D21,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0x1C</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="7">
-        <v>3</v>
-      </c>
-      <c r="D17" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
-        <v>6C</v>
-      </c>
-      <c r="E17" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
-        <v>CC</v>
-      </c>
-      <c r="F17" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
-        <v>9C</v>
-      </c>
-      <c r="G17" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C17,4)),5,1),2)</f>
-        <v>44</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="7">
-        <v>2</v>
-      </c>
-      <c r="D18" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
-        <v>2C</v>
-      </c>
-      <c r="E18" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
-        <v>0C</v>
-      </c>
-      <c r="F18" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
-        <v>1C</v>
-      </c>
-      <c r="G18" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C18,4)),5,1),2)</f>
-        <v>04</v>
-      </c>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="C22" s="7">
         <v>13</v>
       </c>
-      <c r="D19" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(D$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
+      <c r="D22" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>1101</v>
+      </c>
+      <c r="E22" s="3" t="str">
+        <f>"0x"&amp;BIN2HEX(MID($D$15,4,1)&amp;MID(D22,4,1)&amp;MID($D$15,2,1)&amp;MID(D22,2,1)&amp;MID($D$15,3,1)&amp;MID(D22,3,1)&amp;MID($D$15,1,1)&amp;MID(D22,1,1),2)</f>
+        <v>0x51</v>
+      </c>
+      <c r="F22" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D22,4,1)&amp;MID($D$15,4,1)&amp;MID(D22,2,1)&amp;MID($D$15,2,1)&amp;MID(D22,3,1)&amp;MID($D$15,3,1)&amp;MID(D22,1,1)&amp;MID($D$15,1,1),2)</f>
+        <v>0xA2</v>
+      </c>
+      <c r="G22" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D22,4,1)&amp;MID(D22,4,1)&amp;MID(D22,2,1)&amp;MID(D22,2,1)&amp;MID(D22,3,1)&amp;MID(D22,3,1)&amp;MID(D22,1,1)&amp;MID(D22,1,1),2)</f>
+        <v>0xF3</v>
+      </c>
+      <c r="H22" t="str">
+        <f>"0x"&amp;BIN2HEX(MID(D22,4,1)&amp;MID($D$16,4,1)&amp;MID(D22,2,1)&amp;MID($D$16,2,1)&amp;MID(D22,3,1)&amp;MID($D$16,3,1)&amp;MID(D22,1,1)&amp;MID($D$16,1,1),2)</f>
+        <v>0xB6</v>
+      </c>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(E$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
-        <v>F3</v>
-      </c>
-      <c r="F19" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(F$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
-        <v>B6</v>
-      </c>
-      <c r="G19" s="34" t="str">
-        <f>BIN2HEX(MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),4,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),8,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),2,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),6,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),3,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),7,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),1,1)&amp;MID(SUBSTITUTE(G$13,1111,DEC2BIN($C19,4)),5,1),2)</f>
-        <v>51</v>
-      </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="H20" s="28"/>
-      <c r="I20" s="11"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="11"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="3"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
+      <c r="P24" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="11"/>
-      <c r="L25" s="11"/>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="P25" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q25" s="11"/>
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B26" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="11"/>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
+      <c r="P26" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q26" s="11"/>
       <c r="R26" s="11"/>
       <c r="S26" s="11"/>
       <c r="T26" s="11"/>
       <c r="U26" s="11"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="L27" s="11"/>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
+      <c r="P27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q27" s="11"/>
       <c r="R27" s="11"/>
       <c r="S27" s="11"/>
       <c r="T27" s="11"/>
       <c r="U27" s="11"/>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="L28" s="11"/>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
+      <c r="P28" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="Q28" s="11"/>
       <c r="R28" s="11"/>
       <c r="S28" s="11"/>
       <c r="T28" s="11"/>
       <c r="U28" s="11"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B29" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="L29" s="11"/>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
       <c r="U29" s="11"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="L30" s="11"/>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
       <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
       <c r="U30" s="11"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="L31" s="11"/>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
@@ -1456,65 +1570,21 @@
       <c r="T31" s="11"/>
       <c r="U31" s="11"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-    </row>
-    <row r="33" spans="12:21" x14ac:dyDescent="0.2">
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-    </row>
-    <row r="34" spans="12:21" x14ac:dyDescent="0.2">
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="11"/>
-    </row>
-    <row r="35" spans="12:21" x14ac:dyDescent="0.2">
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
-    </row>
-    <row r="36" spans="12:21" x14ac:dyDescent="0.2">
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
+    <row r="34" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+    </row>
+    <row r="37" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1525,6 +1595,7 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1537,42 +1608,42 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>0</v>
       </c>
@@ -1591,22 +1662,20 @@
       <c r="H4" s="7">
         <v>0</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
       <c r="M4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" t="s">
         <v>16</v>
       </c>
-      <c r="P4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="str">
         <f>DEC2BIN(B4,2)</f>
         <v>00</v>
@@ -1632,39 +1701,39 @@
         <v>0000</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5">
         <v>55</v>
       </c>
       <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
         <v>11</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>12</v>
       </c>
-      <c r="P5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6">
         <v>55</v>
       </c>
       <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" t="s">
         <v>20</v>
       </c>
-      <c r="O6" t="s">
-        <v>21</v>
-      </c>
       <c r="P6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1675,13 +1744,13 @@
         <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="L7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M7">
         <v>10</v>
@@ -1690,13 +1759,13 @@
         <v>35</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="str">
         <f>BIN2HEX(B9,1)</f>
         <v>4</v>
@@ -1705,8 +1774,8 @@
         <f>BIN2HEX(C9,1)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="G8" s="1">
         <f>BIN2DEC(G9)</f>
         <v>0</v>
@@ -1724,321 +1793,318 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B9" s="20" t="str">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="str">
         <f>MID(B5,2,1)&amp;MID(C5,2,1)&amp;MID(D5,2,1)&amp;MID(E5,2,1)</f>
         <v>0100</v>
       </c>
-      <c r="C9" s="20" t="str">
+      <c r="C9" s="18" t="str">
         <f>MID(B5,1,1)&amp;MID(C5,1,1)&amp;MID(D5,1,1)&amp;MID(E5,1,1)</f>
         <v>0000</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="G9" s="20" t="str">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="18" t="str">
         <f>MID(H5,1,1)&amp;MID(G5,1,1)</f>
         <v>00</v>
       </c>
-      <c r="H9" s="20" t="str">
+      <c r="H9" s="18" t="str">
         <f>MID(H5,2,1)&amp;MID(G5,2,1)</f>
         <v>01</v>
       </c>
-      <c r="I9" s="20" t="str">
+      <c r="I9" s="18" t="str">
         <f>MID(H5,3,1)&amp;MID(G5,3,1)</f>
         <v>00</v>
       </c>
-      <c r="J9" s="20" t="str">
+      <c r="J9" s="18" t="str">
         <f>MID(H5,4,1)&amp;MID(G5,4,1)</f>
         <v>00</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="18" t="s">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="G12" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="17">
-        <v>1</v>
-      </c>
-      <c r="D13" s="16" t="str">
+      <c r="I12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="str">
         <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D12,1,$C$13),4,1),2),1,1),2)</f>
         <v>E0</v>
       </c>
-      <c r="E13" s="16" t="str">
-        <f t="shared" ref="E13:M13" si="1">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),4,1),2),1,1),2)</f>
+      <c r="E13" s="14" t="str">
+        <f t="shared" ref="E13:K13" si="1">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E12,1,$C$13),4,1),2),1,1),2)</f>
         <v>C0</v>
       </c>
-      <c r="F13" s="16" t="str">
+      <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>A0</v>
       </c>
-      <c r="G13" s="16" t="str">
+      <c r="G13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="H13" s="16" t="str">
+      <c r="H13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="I13" s="16" t="str">
+      <c r="I13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J13" s="16" t="str">
+      <c r="J13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="K13" s="16" t="str">
+      <c r="K13" s="14" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="V13" s="13"/>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B14" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="17">
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="V13" s="11"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="15">
         <v>2</v>
       </c>
-      <c r="D14" s="16" t="str">
+      <c r="D14" s="14" t="str">
         <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$14),4,1),2),1,1),2)</f>
         <v>0E</v>
       </c>
-      <c r="E14" s="16" t="str">
-        <f t="shared" ref="E14:M14" si="2">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),4,1),2),1,1),2)</f>
+      <c r="E14" s="14" t="str">
+        <f t="shared" ref="E14:K14" si="2">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$14),4,1),2),1,1),2)</f>
         <v>0C</v>
       </c>
-      <c r="F14" s="16" t="str">
+      <c r="F14" s="14" t="str">
         <f t="shared" si="2"/>
         <v>0A</v>
       </c>
-      <c r="G14" s="16" t="str">
+      <c r="G14" s="14" t="str">
         <f t="shared" si="2"/>
         <v>08</v>
       </c>
-      <c r="H14" s="16" t="str">
+      <c r="H14" s="14" t="str">
         <f t="shared" si="2"/>
         <v>06</v>
       </c>
-      <c r="I14" s="16" t="str">
+      <c r="I14" s="14" t="str">
         <f t="shared" si="2"/>
         <v>04</v>
       </c>
-      <c r="J14" s="16" t="str">
+      <c r="J14" s="14" t="str">
         <f t="shared" si="2"/>
         <v>02</v>
       </c>
-      <c r="K14" s="16" t="str">
+      <c r="K14" s="14" t="str">
         <f t="shared" si="2"/>
         <v>00</v>
       </c>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="V14" s="13"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="17">
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="V14" s="11"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="15">
         <v>3</v>
       </c>
-      <c r="D15" s="16" t="str">
+      <c r="D15" s="14" t="str">
         <f>BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(D$12,1,$C$15),4,1),2),1,1),2)</f>
         <v>EE</v>
       </c>
-      <c r="E15" s="16" t="str">
-        <f t="shared" ref="E15:L15" si="3">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),4,1),2),1,1),2)</f>
+      <c r="E15" s="14" t="str">
+        <f t="shared" ref="E15:K15" si="3">BIN2HEX(MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),1,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),2,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),3,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),4,1),2),2,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),1,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),2,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),3,1),2),1,1)&amp;MID(DEC2BIN(MID(SUBSTITUTE(E$12,1,$C$15),4,1),2),1,1),2)</f>
         <v>CC</v>
       </c>
-      <c r="F15" s="16" t="str">
+      <c r="F15" s="14" t="str">
         <f t="shared" si="3"/>
         <v>AA</v>
       </c>
-      <c r="G15" s="16" t="str">
+      <c r="G15" s="14" t="str">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="H15" s="16" t="str">
+      <c r="H15" s="14" t="str">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
-      <c r="I15" s="16" t="str">
+      <c r="I15" s="14" t="str">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="J15" s="16" t="str">
+      <c r="J15" s="14" t="str">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="K15" s="16" t="str">
+      <c r="K15" s="14" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="V15" s="13"/>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="V15" s="11"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="V16" s="13"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="V16" s="11"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="V17" s="11"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="V17" s="13"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="V18" s="11"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="V18" s="13"/>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="V19" s="11"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="V19" s="13"/>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B21" s="12" t="s">
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B23" s="12" t="s">
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B25" s="12" t="s">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B26" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>1</v>
       </c>
@@ -2052,7 +2118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>1</v>
       </c>
@@ -2066,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>1</v>
       </c>
@@ -2080,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>1</v>
       </c>
@@ -2094,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>1</v>
       </c>
@@ -2108,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1</v>
       </c>
@@ -2122,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>1</v>
       </c>
@@ -2136,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>1</v>
       </c>
@@ -2150,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>1</v>
       </c>
@@ -2164,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0</v>
       </c>
@@ -2178,101 +2244,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="13">
-        <v>0</v>
-      </c>
-      <c r="C38" s="13">
-        <v>1</v>
-      </c>
-      <c r="D38" s="13">
-        <v>1</v>
-      </c>
-      <c r="E38" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="13">
-        <v>0</v>
-      </c>
-      <c r="C39" s="13">
-        <v>1</v>
-      </c>
-      <c r="D39" s="13">
-        <v>0</v>
-      </c>
-      <c r="E39" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="13">
-        <v>0</v>
-      </c>
-      <c r="C40" s="13">
-        <v>1</v>
-      </c>
-      <c r="D40" s="13">
-        <v>0</v>
-      </c>
-      <c r="E40" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="13">
-        <v>0</v>
-      </c>
-      <c r="C41" s="13">
-        <v>0</v>
-      </c>
-      <c r="D41" s="13">
-        <v>1</v>
-      </c>
-      <c r="E41" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="13">
-        <v>0</v>
-      </c>
-      <c r="C42" s="13">
-        <v>0</v>
-      </c>
-      <c r="D42" s="13">
-        <v>1</v>
-      </c>
-      <c r="E42" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="13">
-        <v>0</v>
-      </c>
-      <c r="C43" s="13">
-        <v>0</v>
-      </c>
-      <c r="D43" s="13">
-        <v>0</v>
-      </c>
-      <c r="E43" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="13">
-        <v>0</v>
-      </c>
-      <c r="C44" s="13">
-        <v>0</v>
-      </c>
-      <c r="D44" s="13">
-        <v>0</v>
-      </c>
-      <c r="E44" s="13">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <v>0</v>
+      </c>
+      <c r="C38" s="11">
+        <v>1</v>
+      </c>
+      <c r="D38" s="11">
+        <v>1</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <v>0</v>
+      </c>
+      <c r="C39" s="11">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11">
+        <v>0</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
+        <v>0</v>
+      </c>
+      <c r="C40" s="11">
+        <v>1</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="11">
+        <v>0</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0</v>
+      </c>
+      <c r="D41" s="11">
+        <v>1</v>
+      </c>
+      <c r="E41" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>0</v>
+      </c>
+      <c r="C42" s="11">
+        <v>0</v>
+      </c>
+      <c r="D42" s="11">
+        <v>1</v>
+      </c>
+      <c r="E42" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11">
+        <v>0</v>
+      </c>
+      <c r="C43" s="11">
+        <v>0</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0</v>
+      </c>
+      <c r="E43" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <v>0</v>
+      </c>
+      <c r="C44" s="11">
+        <v>0</v>
+      </c>
+      <c r="D44" s="11">
+        <v>0</v>
+      </c>
+      <c r="E44" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2298,7 +2364,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>